<commit_message>
configured selenium grid set-up, standalone
</commit_message>
<xml_diff>
--- a/TestData/Testdata.xlsx
+++ b/TestData/Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\eclipse-workspace\EcommerceApp\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437FE1D4-C47D-47E3-8E64-B524D54AE410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD04CEB-4591-4C3D-859F-E81AC838295D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{228D4D4B-2128-4EC8-9A58-F0C1B08F6BD9}"/>
   </bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,7 +522,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.4">
@@ -533,7 +533,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.4">

</xml_diff>